<commit_message>
Methods to Check DSP Channel mapping
</commit_message>
<xml_diff>
--- a/AutoFirmwareUpgrade/ClassLibrary1/TestDataFiles/CablingDataSet/3U_Standalone.xlsx
+++ b/AutoFirmwareUpgrade/ClassLibrary1/TestDataFiles/CablingDataSet/3U_Standalone.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4299FA7A-2879-4687-9DCB-8CF59066237E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682CB5C8-755A-4EE2-A49D-23EFA776AC3C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DeviceInfo" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="81">
   <si>
     <t>Channel</t>
   </si>
@@ -231,9 +231,6 @@
     <t>usage</t>
   </si>
   <si>
-    <t>Channel Number</t>
-  </si>
-  <si>
     <t>PMP_FR_Cabling</t>
   </si>
   <si>
@@ -262,6 +259,12 @@
   </si>
   <si>
     <t>sn409026540_3U_15I.cal</t>
+  </si>
+  <si>
+    <t>Channel_Number_DSP1</t>
+  </si>
+  <si>
+    <t>Channel_Number_DSP2</t>
   </si>
 </sst>
 </file>
@@ -581,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC80E08-4779-41B6-BC5C-D4F1EB97A33C}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
@@ -593,18 +596,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
         <v>76</v>
-      </c>
-      <c r="B1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
         <v>78</v>
-      </c>
-      <c r="B2" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -617,8 +620,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +629,7 @@
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
@@ -669,10 +672,10 @@
         <v>68</v>
       </c>
       <c r="K1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" t="s">
         <v>70</v>
-      </c>
-      <c r="L1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -707,10 +710,10 @@
         <v>28</v>
       </c>
       <c r="K2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -785,7 +788,7 @@
         <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>66</v>
@@ -797,7 +800,7 @@
         <v>67</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -817,7 +820,7 @@
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>66</v>
@@ -829,7 +832,7 @@
         <v>67</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -867,7 +870,7 @@
         <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>66</v>
@@ -879,7 +882,7 @@
         <v>67</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -917,7 +920,7 @@
         <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
         <v>66</v>
@@ -964,7 +967,7 @@
         <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>66</v>
@@ -1011,7 +1014,7 @@
         <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>66</v>
@@ -1055,7 +1058,7 @@
         <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
         <v>66</v>
@@ -1093,7 +1096,7 @@
         <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
         <v>66</v>
@@ -1128,7 +1131,7 @@
         <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
         <v>66</v>
@@ -1163,7 +1166,7 @@
         <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
         <v>66</v>
@@ -1198,7 +1201,7 @@
         <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
         <v>66</v>
@@ -1233,7 +1236,7 @@
         <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
         <v>66</v>
@@ -1268,7 +1271,7 @@
         <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
         <v>66</v>
@@ -1303,7 +1306,7 @@
         <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
         <v>66</v>
@@ -1338,7 +1341,7 @@
         <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
         <v>66</v>
@@ -1417,29 +1420,29 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B13"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" t="s">
-        <v>73</v>
-      </c>
       <c r="D1" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>